<commit_message>
Squashed a bunch of commits that were the result of transferring code changes between clones.
</commit_message>
<xml_diff>
--- a/DataRepo/example_data/test_dataframes/animal_sample_table_df_test1.xlsx
+++ b/DataRepo/example_data/test_dataframes/animal_sample_table_df_test1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fkang/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rleach/PROJECT-LOCAL/TRACEBASE/tracebase/DataRepo/example_data/test_dataframes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44DDC3ED-0F3B-8541-A553-F48D7AC2D5A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{9A34FFDF-BEFE-A64D-A356-73597741F8D5}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5300" yWindow="500" windowWidth="56100" windowHeight="21100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="21100" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Animals" sheetId="1" r:id="rId1"/>
@@ -1123,7 +1123,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMJ952"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
+    <sheetView zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
@@ -5198,14 +5198,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AD399"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="26.83203125" customWidth="1"/>
+    <col min="1" max="1" width="14.5" customWidth="1"/>
     <col min="3" max="3" width="20.5" customWidth="1"/>
     <col min="4" max="4" width="31.5" customWidth="1"/>
     <col min="5" max="5" width="15.33203125" customWidth="1"/>

</xml_diff>